<commit_message>
Simpler model without OPF constraints or risk
Simpler model without OPF constraints or risk. Missing the lambdas
</commit_message>
<xml_diff>
--- a/DA_prices.xlsx
+++ b/DA_prices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/de7c5f4e9a006291/Documents/Optimisation in MS/assignement/optimization_code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Opti in modern power systems\code\optimization_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{858434A4-DE73-4F4D-AD91-D092A24486C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9D15EF5-8339-4621-B7BD-B429577319DA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858434A4-DE73-4F4D-AD91-D092A24486C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -92,10 +92,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -361,258 +357,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B25"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="1">
+        <v>50.81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>1+A2</f>
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="1">
+        <v>51.51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A25" si="0">1+A3</f>
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="1">
+        <v>51.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <v>51.91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <v>52.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>52.52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <v>54.46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <v>58.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>59.94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <v>59.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>59.94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <v>57.98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>54.11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>56.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>66.72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>72.209999999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>78.28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>89.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
+        <v>93.73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
+        <v>87.19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="1">
+        <v>77.489999999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
+        <v>71.62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <v>70.06</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1"/>
+      <c r="B25" s="1">
+        <v>66.39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>